<commit_message>
modified:   Survey_data.xlsx 	renamed:    code/get Species_list.py -> code/get_Species_list.py
</commit_message>
<xml_diff>
--- a/Survey_data.xlsx
+++ b/Survey_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awilhelm/Desktop/grad_school/TFCB2023/tfcb-homework01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BCDBC2-A046-1B4F-83CB-DD5429D2751D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89E3588-B615-E844-9990-612120F7CE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="4120" windowWidth="25120" windowHeight="15580" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -86,9 +86,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,7 +162,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,7 +562,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -606,7 +606,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -631,10 +631,10 @@
   <dimension ref="A1:AE50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C3" sqref="C3:C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1"/>
@@ -656,7 +656,7 @@
     <col min="32" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="30">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="3"/>
@@ -678,7 +678,7 @@
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="30">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="30">
       <c r="A3" s="8">
         <v>2013</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="30">
       <c r="A4" s="8">
         <v>2013</v>
       </c>
@@ -786,7 +786,7 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="30">
       <c r="A5" s="8">
         <v>2013</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="30">
       <c r="A6" s="8">
         <v>2013</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="30">
       <c r="A7" s="8">
         <v>2013</v>
       </c>
@@ -894,7 +894,7 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="8">
         <v>2013</v>
       </c>
@@ -930,7 +930,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="30">
       <c r="A9" s="8">
         <v>2013</v>
       </c>
@@ -966,7 +966,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="30">
       <c r="A10" s="8">
         <v>2013</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="30">
       <c r="A11" s="8">
         <v>2013</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="30">
       <c r="A12" s="8">
         <v>2013</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="30">
       <c r="A13" s="8">
         <v>2013</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="30">
       <c r="A14" s="8">
         <v>2013</v>
       </c>
@@ -1142,7 +1142,7 @@
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
-    <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="30">
       <c r="A15" s="8">
         <v>2013</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
     </row>
-    <row r="16" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="30">
       <c r="A16" s="8">
         <v>2013</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
     </row>
-    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="30">
       <c r="A17" s="8">
         <v>2013</v>
       </c>
@@ -1247,7 +1247,7 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
     </row>
-    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="30">
       <c r="A18" s="8">
         <v>2013</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="30">
       <c r="A19" s="8">
         <v>2013</v>
       </c>
@@ -1307,7 +1307,7 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
     </row>
-    <row r="20" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="30">
       <c r="A20" s="8">
         <v>2013</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="N20" s="4"/>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="30">
       <c r="A21" s="8">
         <v>2013</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="N21" s="4"/>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="30">
       <c r="A22" s="8">
         <v>2013</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="N22" s="4"/>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="30">
       <c r="A23" s="8">
         <v>2013</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="N23" s="4"/>
       <c r="T23" s="4"/>
     </row>
-    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="30">
       <c r="A24" s="8">
         <v>2014</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="30">
       <c r="A25" s="8">
         <v>2014</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="30">
       <c r="A26" s="8">
         <v>2014</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="30">
       <c r="A27" s="8">
         <v>2014</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="30">
       <c r="A28" s="8">
         <v>2014</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="30">
       <c r="A29" s="8">
         <v>2014</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="30">
       <c r="A30" s="8">
         <v>2014</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="30">
       <c r="A31" s="8">
         <v>2014</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="30">
       <c r="A32" s="8">
         <v>2014</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="30">
       <c r="A33" s="8">
         <v>2014</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="30">
       <c r="A34" s="8">
         <v>2014</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="30">
       <c r="A35" s="8">
         <v>2014</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="30">
       <c r="A36" s="8">
         <v>2014</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="30">
       <c r="A37" s="8">
         <v>2014</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="30">
       <c r="A38" s="8">
         <v>2014</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="30">
       <c r="A39" s="8">
         <v>2014</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="30">
       <c r="A40" s="8">
         <v>2014</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="30">
       <c r="A41" s="8">
         <v>2014</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30">
       <c r="A42" s="8">
         <v>2014</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="30">
       <c r="A43" s="8">
         <v>2014</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="30">
       <c r="A44" s="8">
         <v>2014</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="30">
       <c r="A45" s="8">
         <v>2014</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="30">
       <c r="A46" s="8">
         <v>2014</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="30">
       <c r="A47" s="8">
         <v>2014</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="30">
       <c r="A48" s="8">
         <v>2014</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="30">
       <c r="A49" s="8">
         <v>2014</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="30">
       <c r="A50" s="8">
         <v>2014</v>
       </c>

</xml_diff>